<commit_message>
fixed import_metadat_dat method to use shlex to be format agnositc to process old dats, added a few patches, updated libretro-db
</commit_message>
<xml_diff>
--- a/patches.xlsx
+++ b/patches.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$N$470</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$N$471</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4607" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4616" uniqueCount="208">
   <si>
     <t>Action</t>
   </si>
@@ -648,6 +648,9 @@
   </si>
   <si>
     <t>SoftwareFlagMap</t>
+  </si>
+  <si>
+    <t>'/jaguar/918759-international-sensible-soccer'</t>
   </si>
 </sst>
 </file>
@@ -1001,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N470"/>
+  <dimension ref="A1:N471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1026,7 @@
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="64.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1066,7 +1069,7 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1739,7 +1742,7 @@
       <c r="M40" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1766,7 +1769,7 @@
       <c r="M41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1793,7 +1796,7 @@
       <c r="M42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1820,7 +1823,7 @@
       <c r="M43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1884,7 +1887,7 @@
       <c r="M45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1916,7 +1919,7 @@
       <c r="M46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1948,7 +1951,7 @@
       <c r="M47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N47" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1980,7 +1983,7 @@
       <c r="M48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N48" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2006,14 +2009,14 @@
       <c r="J49" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K49">
-        <v>323</v>
+      <c r="K49" s="2">
+        <v>210</v>
       </c>
       <c r="M49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N49" t="s">
-        <v>34</v>
+      <c r="N49" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -2039,13 +2042,13 @@
         <v>202</v>
       </c>
       <c r="K50">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N50" t="s">
-        <v>35</v>
+      <c r="N50" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -2071,13 +2074,13 @@
         <v>202</v>
       </c>
       <c r="K51">
-        <v>460</v>
+        <v>325</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N51" t="s">
-        <v>36</v>
+      <c r="N51" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -2103,13 +2106,13 @@
         <v>202</v>
       </c>
       <c r="K52">
-        <v>772</v>
+        <v>460</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N52" t="s">
-        <v>37</v>
+      <c r="N52" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -2135,13 +2138,13 @@
         <v>202</v>
       </c>
       <c r="K53">
-        <v>779</v>
+        <v>772</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N53" t="s">
-        <v>38</v>
+      <c r="N53" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -2166,14 +2169,14 @@
       <c r="J54" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K54" s="2">
-        <v>780</v>
+      <c r="K54">
+        <v>779</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N54" t="s">
-        <v>39</v>
+      <c r="N54" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -2199,13 +2202,13 @@
         <v>202</v>
       </c>
       <c r="K55" s="2">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N55" t="s">
-        <v>40</v>
+      <c r="N55" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -2231,13 +2234,13 @@
         <v>202</v>
       </c>
       <c r="K56" s="2">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N56" t="s">
-        <v>41</v>
+      <c r="N56" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -2263,13 +2266,13 @@
         <v>202</v>
       </c>
       <c r="K57" s="2">
-        <v>809</v>
+        <v>782</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N57" t="s">
-        <v>42</v>
+      <c r="N57" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -2295,13 +2298,13 @@
         <v>202</v>
       </c>
       <c r="K58" s="2">
-        <v>1000</v>
+        <v>809</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N58" t="s">
-        <v>43</v>
+      <c r="N58" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -2327,13 +2330,13 @@
         <v>202</v>
       </c>
       <c r="K59" s="2">
-        <v>1015</v>
+        <v>1000</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N59" t="s">
-        <v>44</v>
+      <c r="N59" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -2359,13 +2362,13 @@
         <v>202</v>
       </c>
       <c r="K60" s="2">
-        <v>1041</v>
+        <v>1015</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N60" t="s">
-        <v>45</v>
+      <c r="N60" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -2391,13 +2394,13 @@
         <v>202</v>
       </c>
       <c r="K61" s="2">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N61" t="s">
-        <v>46</v>
+      <c r="N61" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -2423,13 +2426,13 @@
         <v>202</v>
       </c>
       <c r="K62" s="2">
-        <v>1047</v>
+        <v>1042</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N62" t="s">
-        <v>47</v>
+      <c r="N62" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -2455,13 +2458,13 @@
         <v>202</v>
       </c>
       <c r="K63" s="2">
-        <v>1071</v>
+        <v>1047</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N63" t="s">
-        <v>48</v>
+      <c r="N63" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -2487,13 +2490,13 @@
         <v>202</v>
       </c>
       <c r="K64" s="2">
-        <v>1078</v>
+        <v>1071</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N64" t="s">
-        <v>49</v>
+      <c r="N64" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -2518,14 +2521,14 @@
       <c r="J65" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K65">
-        <v>1091</v>
+      <c r="K65" s="2">
+        <v>1078</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N65" t="s">
-        <v>50</v>
+      <c r="N65" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -2551,13 +2554,13 @@
         <v>202</v>
       </c>
       <c r="K66">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N66" t="s">
-        <v>51</v>
+      <c r="N66" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -2583,13 +2586,13 @@
         <v>202</v>
       </c>
       <c r="K67">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="M67" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N67" t="s">
-        <v>52</v>
+      <c r="N67" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -2615,13 +2618,13 @@
         <v>202</v>
       </c>
       <c r="K68">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N68" t="s">
-        <v>53</v>
+      <c r="N68" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -2647,13 +2650,13 @@
         <v>202</v>
       </c>
       <c r="K69">
-        <v>1108</v>
+        <v>1103</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N69" t="s">
-        <v>54</v>
+      <c r="N69" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -2679,13 +2682,13 @@
         <v>202</v>
       </c>
       <c r="K70">
-        <v>1122</v>
+        <v>1108</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N70" t="s">
-        <v>55</v>
+      <c r="N70" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -2711,13 +2714,13 @@
         <v>202</v>
       </c>
       <c r="K71">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N71" t="s">
-        <v>56</v>
+      <c r="N71" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -2743,13 +2746,13 @@
         <v>202</v>
       </c>
       <c r="K72">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N72" t="s">
-        <v>57</v>
+      <c r="N72" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -2775,13 +2778,13 @@
         <v>202</v>
       </c>
       <c r="K73">
-        <v>1142</v>
+        <v>1124</v>
       </c>
       <c r="M73" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N73" t="s">
-        <v>58</v>
+      <c r="N73" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -2807,13 +2810,13 @@
         <v>202</v>
       </c>
       <c r="K74">
-        <v>1186</v>
+        <v>1142</v>
       </c>
       <c r="M74" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N74" t="s">
-        <v>59</v>
+      <c r="N74" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -2839,13 +2842,13 @@
         <v>202</v>
       </c>
       <c r="K75">
-        <v>1266</v>
+        <v>1186</v>
       </c>
       <c r="M75" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N75" t="s">
-        <v>60</v>
+      <c r="N75" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -2871,13 +2874,13 @@
         <v>202</v>
       </c>
       <c r="K76">
-        <v>1342</v>
+        <v>1266</v>
       </c>
       <c r="M76" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N76" t="s">
-        <v>61</v>
+      <c r="N76" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -2903,13 +2906,13 @@
         <v>202</v>
       </c>
       <c r="K77">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="M77" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N77" t="s">
-        <v>62</v>
+      <c r="N77" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -2935,13 +2938,13 @@
         <v>202</v>
       </c>
       <c r="K78">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="M78" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N78" t="s">
-        <v>63</v>
+      <c r="N78" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -2967,13 +2970,13 @@
         <v>202</v>
       </c>
       <c r="K79">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="M79" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N79" t="s">
-        <v>64</v>
+      <c r="N79" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -2999,13 +3002,13 @@
         <v>202</v>
       </c>
       <c r="K80">
-        <v>1378</v>
+        <v>1358</v>
       </c>
       <c r="M80" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N80" t="s">
-        <v>65</v>
+      <c r="N80" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -3031,13 +3034,13 @@
         <v>202</v>
       </c>
       <c r="K81">
-        <v>1394</v>
+        <v>1378</v>
       </c>
       <c r="M81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N81" t="s">
-        <v>66</v>
+      <c r="N81" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -3063,13 +3066,13 @@
         <v>202</v>
       </c>
       <c r="K82">
-        <v>1413</v>
+        <v>1394</v>
       </c>
       <c r="M82" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N82" t="s">
-        <v>67</v>
+      <c r="N82" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -3095,13 +3098,13 @@
         <v>202</v>
       </c>
       <c r="K83">
-        <v>1425</v>
+        <v>1413</v>
       </c>
       <c r="M83" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N83" t="s">
-        <v>68</v>
+      <c r="N83" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -3127,13 +3130,13 @@
         <v>202</v>
       </c>
       <c r="K84">
-        <v>1802</v>
+        <v>1425</v>
       </c>
       <c r="M84" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N84" t="s">
-        <v>69</v>
+      <c r="N84" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -3159,13 +3162,13 @@
         <v>202</v>
       </c>
       <c r="K85">
-        <v>1871</v>
+        <v>1802</v>
       </c>
       <c r="M85" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N85" t="s">
-        <v>70</v>
+      <c r="N85" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -3191,13 +3194,13 @@
         <v>202</v>
       </c>
       <c r="K86">
-        <v>1885</v>
+        <v>1871</v>
       </c>
       <c r="M86" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N86" t="s">
-        <v>71</v>
+      <c r="N86" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -3223,13 +3226,13 @@
         <v>202</v>
       </c>
       <c r="K87">
-        <v>2027</v>
+        <v>1885</v>
       </c>
       <c r="M87" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N87" t="s">
-        <v>72</v>
+      <c r="N87" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -3255,13 +3258,13 @@
         <v>202</v>
       </c>
       <c r="K88">
-        <v>2322</v>
+        <v>2027</v>
       </c>
       <c r="M88" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N88" t="s">
-        <v>73</v>
+      <c r="N88" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -3287,13 +3290,13 @@
         <v>202</v>
       </c>
       <c r="K89">
-        <v>2393</v>
+        <v>2322</v>
       </c>
       <c r="M89" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N89" t="s">
-        <v>74</v>
+      <c r="N89" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -3319,13 +3322,13 @@
         <v>202</v>
       </c>
       <c r="K90">
-        <v>2417</v>
+        <v>2393</v>
       </c>
       <c r="M90" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N90" t="s">
-        <v>75</v>
+      <c r="N90" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -3351,13 +3354,13 @@
         <v>202</v>
       </c>
       <c r="K91">
-        <v>2574</v>
+        <v>2417</v>
       </c>
       <c r="M91" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N91" t="s">
-        <v>76</v>
+      <c r="N91" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -3383,13 +3386,13 @@
         <v>202</v>
       </c>
       <c r="K92">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="M92" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N92" t="s">
-        <v>77</v>
+      <c r="N92" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -3415,13 +3418,13 @@
         <v>202</v>
       </c>
       <c r="K93">
-        <v>2627</v>
+        <v>2575</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N93" t="s">
-        <v>78</v>
+      <c r="N93" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -3447,13 +3450,13 @@
         <v>202</v>
       </c>
       <c r="K94">
-        <v>2756</v>
+        <v>2627</v>
       </c>
       <c r="M94" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N94" t="s">
-        <v>79</v>
+      <c r="N94" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -3479,13 +3482,13 @@
         <v>202</v>
       </c>
       <c r="K95">
-        <v>2815</v>
+        <v>2756</v>
       </c>
       <c r="M95" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N95" t="s">
-        <v>80</v>
+      <c r="N95" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -3511,13 +3514,13 @@
         <v>202</v>
       </c>
       <c r="K96">
-        <v>2943</v>
+        <v>2815</v>
       </c>
       <c r="M96" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N96" t="s">
-        <v>81</v>
+      <c r="N96" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -3543,13 +3546,13 @@
         <v>202</v>
       </c>
       <c r="K97">
-        <v>3006</v>
+        <v>2943</v>
       </c>
       <c r="M97" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N97" t="s">
-        <v>82</v>
+      <c r="N97" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -3575,13 +3578,13 @@
         <v>202</v>
       </c>
       <c r="K98">
-        <v>3038</v>
+        <v>3006</v>
       </c>
       <c r="M98" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N98" t="s">
-        <v>83</v>
+      <c r="N98" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -3607,13 +3610,13 @@
         <v>202</v>
       </c>
       <c r="K99">
-        <v>3134</v>
+        <v>3038</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N99" t="s">
-        <v>84</v>
+      <c r="N99" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -3639,13 +3642,13 @@
         <v>202</v>
       </c>
       <c r="K100">
-        <v>3213</v>
+        <v>3134</v>
       </c>
       <c r="M100" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N100" t="s">
-        <v>85</v>
+      <c r="N100" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -3671,13 +3674,13 @@
         <v>202</v>
       </c>
       <c r="K101">
-        <v>3432</v>
+        <v>3213</v>
       </c>
       <c r="M101" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N101" t="s">
-        <v>86</v>
+      <c r="N101" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -3703,13 +3706,13 @@
         <v>202</v>
       </c>
       <c r="K102">
-        <v>3563</v>
+        <v>3432</v>
       </c>
       <c r="M102" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N102" t="s">
-        <v>87</v>
+      <c r="N102" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -3735,13 +3738,13 @@
         <v>202</v>
       </c>
       <c r="K103">
-        <v>3598</v>
+        <v>3563</v>
       </c>
       <c r="M103" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N103" t="s">
-        <v>88</v>
+      <c r="N103" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -3767,13 +3770,13 @@
         <v>202</v>
       </c>
       <c r="K104">
-        <v>3660</v>
+        <v>3598</v>
       </c>
       <c r="M104" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N104" t="s">
-        <v>89</v>
+      <c r="N104" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -3799,13 +3802,13 @@
         <v>202</v>
       </c>
       <c r="K105">
-        <v>3666</v>
+        <v>3660</v>
       </c>
       <c r="M105" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N105" t="s">
-        <v>90</v>
+      <c r="N105" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -3831,13 +3834,13 @@
         <v>202</v>
       </c>
       <c r="K106">
-        <v>3729</v>
+        <v>3666</v>
       </c>
       <c r="M106" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N106" t="s">
-        <v>91</v>
+      <c r="N106" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -3863,13 +3866,13 @@
         <v>202</v>
       </c>
       <c r="K107">
-        <v>3887</v>
+        <v>3729</v>
       </c>
       <c r="M107" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N107" t="s">
-        <v>92</v>
+      <c r="N107" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -3895,13 +3898,13 @@
         <v>202</v>
       </c>
       <c r="K108">
-        <v>4013</v>
+        <v>3887</v>
       </c>
       <c r="M108" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N108" t="s">
-        <v>93</v>
+      <c r="N108" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -3927,13 +3930,13 @@
         <v>202</v>
       </c>
       <c r="K109">
-        <v>4223</v>
+        <v>4013</v>
       </c>
       <c r="M109" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N109" t="s">
-        <v>94</v>
+      <c r="N109" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -3959,13 +3962,13 @@
         <v>202</v>
       </c>
       <c r="K110">
-        <v>4379</v>
+        <v>4223</v>
       </c>
       <c r="M110" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N110" t="s">
-        <v>95</v>
+      <c r="N110" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -3991,13 +3994,13 @@
         <v>202</v>
       </c>
       <c r="K111">
-        <v>4460</v>
+        <v>4379</v>
       </c>
       <c r="M111" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N111" t="s">
-        <v>96</v>
+      <c r="N111" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -4023,13 +4026,13 @@
         <v>202</v>
       </c>
       <c r="K112">
-        <v>4527</v>
+        <v>4460</v>
       </c>
       <c r="M112" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N112" t="s">
-        <v>97</v>
+      <c r="N112" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -4055,13 +4058,13 @@
         <v>202</v>
       </c>
       <c r="K113">
-        <v>4555</v>
+        <v>4527</v>
       </c>
       <c r="M113" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N113" t="s">
-        <v>98</v>
+      <c r="N113" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -4087,13 +4090,13 @@
         <v>202</v>
       </c>
       <c r="K114">
-        <v>4592</v>
+        <v>4555</v>
       </c>
       <c r="M114" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N114" t="s">
-        <v>99</v>
+      <c r="N114" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -4119,13 +4122,13 @@
         <v>202</v>
       </c>
       <c r="K115">
-        <v>4819</v>
+        <v>4592</v>
       </c>
       <c r="M115" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N115" t="s">
-        <v>100</v>
+      <c r="N115" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -4151,13 +4154,13 @@
         <v>202</v>
       </c>
       <c r="K116">
-        <v>4823</v>
+        <v>4819</v>
       </c>
       <c r="M116" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N116" t="s">
-        <v>101</v>
+      <c r="N116" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -4183,13 +4186,13 @@
         <v>202</v>
       </c>
       <c r="K117">
-        <v>4831</v>
+        <v>4823</v>
       </c>
       <c r="M117" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N117" t="s">
-        <v>102</v>
+      <c r="N117" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -4215,12 +4218,12 @@
         <v>202</v>
       </c>
       <c r="K118">
-        <v>4832</v>
+        <v>4831</v>
       </c>
       <c r="M118" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N118" t="s">
+      <c r="N118" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4247,13 +4250,13 @@
         <v>202</v>
       </c>
       <c r="K119">
-        <v>4920</v>
+        <v>4832</v>
       </c>
       <c r="M119" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N119" t="s">
-        <v>103</v>
+      <c r="N119" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -4279,13 +4282,13 @@
         <v>202</v>
       </c>
       <c r="K120">
-        <v>4921</v>
+        <v>4920</v>
       </c>
       <c r="M120" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N120" t="s">
-        <v>104</v>
+      <c r="N120" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -4311,13 +4314,13 @@
         <v>202</v>
       </c>
       <c r="K121">
-        <v>4922</v>
+        <v>4921</v>
       </c>
       <c r="M121" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N121" t="s">
-        <v>105</v>
+      <c r="N121" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -4343,13 +4346,13 @@
         <v>202</v>
       </c>
       <c r="K122">
-        <v>5150</v>
+        <v>4922</v>
       </c>
       <c r="M122" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N122" t="s">
-        <v>106</v>
+      <c r="N122" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -4375,13 +4378,13 @@
         <v>202</v>
       </c>
       <c r="K123">
-        <v>5147</v>
+        <v>5150</v>
       </c>
       <c r="M123" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N123" t="s">
-        <v>107</v>
+      <c r="N123" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
@@ -4407,13 +4410,13 @@
         <v>202</v>
       </c>
       <c r="K124">
-        <v>5323</v>
+        <v>5147</v>
       </c>
       <c r="M124" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N124" t="s">
-        <v>108</v>
+      <c r="N124" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -4439,13 +4442,13 @@
         <v>202</v>
       </c>
       <c r="K125">
-        <v>5712</v>
+        <v>5323</v>
       </c>
       <c r="M125" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N125" t="s">
-        <v>109</v>
+      <c r="N125" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -4471,13 +4474,13 @@
         <v>202</v>
       </c>
       <c r="K126">
-        <v>5900</v>
+        <v>5712</v>
       </c>
       <c r="M126" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N126" t="s">
-        <v>110</v>
+      <c r="N126" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -4503,13 +4506,13 @@
         <v>202</v>
       </c>
       <c r="K127">
-        <v>6009</v>
+        <v>5900</v>
       </c>
       <c r="M127" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N127" t="s">
-        <v>111</v>
+      <c r="N127" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -4535,13 +4538,13 @@
         <v>202</v>
       </c>
       <c r="K128">
-        <v>6208</v>
+        <v>6009</v>
       </c>
       <c r="M128" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N128" t="s">
-        <v>112</v>
+      <c r="N128" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -4567,13 +4570,13 @@
         <v>202</v>
       </c>
       <c r="K129">
-        <v>6830</v>
+        <v>6208</v>
       </c>
       <c r="M129" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N129" t="s">
-        <v>113</v>
+      <c r="N129" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
@@ -4599,13 +4602,13 @@
         <v>202</v>
       </c>
       <c r="K130">
-        <v>7492</v>
+        <v>6830</v>
       </c>
       <c r="M130" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N130" t="s">
-        <v>114</v>
+      <c r="N130" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -4631,13 +4634,13 @@
         <v>202</v>
       </c>
       <c r="K131">
-        <v>7491</v>
+        <v>7492</v>
       </c>
       <c r="M131" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N131" t="s">
-        <v>115</v>
+      <c r="N131" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -4663,13 +4666,13 @@
         <v>202</v>
       </c>
       <c r="K132">
-        <v>7494</v>
+        <v>7491</v>
       </c>
       <c r="M132" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N132" t="s">
-        <v>116</v>
+      <c r="N132" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
@@ -4695,13 +4698,13 @@
         <v>202</v>
       </c>
       <c r="K133">
-        <v>7633</v>
+        <v>7494</v>
       </c>
       <c r="M133" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N133" t="s">
-        <v>117</v>
+      <c r="N133" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
@@ -4727,13 +4730,13 @@
         <v>202</v>
       </c>
       <c r="K134">
-        <v>7634</v>
+        <v>7633</v>
       </c>
       <c r="M134" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N134" t="s">
-        <v>118</v>
+      <c r="N134" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -4759,13 +4762,13 @@
         <v>202</v>
       </c>
       <c r="K135">
-        <v>7635</v>
+        <v>7634</v>
       </c>
       <c r="M135" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N135" t="s">
-        <v>119</v>
+      <c r="N135" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
@@ -4791,13 +4794,13 @@
         <v>202</v>
       </c>
       <c r="K136">
-        <v>7636</v>
+        <v>7635</v>
       </c>
       <c r="M136" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N136" t="s">
-        <v>120</v>
+      <c r="N136" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -4823,13 +4826,13 @@
         <v>202</v>
       </c>
       <c r="K137">
-        <v>7637</v>
+        <v>7636</v>
       </c>
       <c r="M137" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N137" t="s">
-        <v>121</v>
+      <c r="N137" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -4855,13 +4858,13 @@
         <v>202</v>
       </c>
       <c r="K138">
-        <v>7837</v>
+        <v>7637</v>
       </c>
       <c r="M138" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N138" t="s">
-        <v>122</v>
+      <c r="N138" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -4887,13 +4890,13 @@
         <v>202</v>
       </c>
       <c r="K139">
-        <v>8000</v>
+        <v>7837</v>
       </c>
       <c r="M139" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N139" t="s">
-        <v>123</v>
+      <c r="N139" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
@@ -4919,13 +4922,13 @@
         <v>202</v>
       </c>
       <c r="K140">
-        <v>8415</v>
+        <v>8000</v>
       </c>
       <c r="M140" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N140" t="s">
-        <v>124</v>
+      <c r="N140" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -4951,13 +4954,13 @@
         <v>202</v>
       </c>
       <c r="K141">
-        <v>8500</v>
+        <v>8415</v>
       </c>
       <c r="M141" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N141" t="s">
-        <v>125</v>
+      <c r="N141" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.25">
@@ -4983,13 +4986,13 @@
         <v>202</v>
       </c>
       <c r="K142">
-        <v>8627</v>
+        <v>8500</v>
       </c>
       <c r="M142" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N142" t="s">
-        <v>126</v>
+      <c r="N142" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
@@ -5015,13 +5018,13 @@
         <v>202</v>
       </c>
       <c r="K143">
-        <v>8860</v>
+        <v>8627</v>
       </c>
       <c r="M143" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N143" t="s">
-        <v>127</v>
+      <c r="N143" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -5047,13 +5050,13 @@
         <v>202</v>
       </c>
       <c r="K144">
-        <v>8946</v>
+        <v>8860</v>
       </c>
       <c r="M144" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N144" t="s">
-        <v>128</v>
+      <c r="N144" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -5079,13 +5082,13 @@
         <v>202</v>
       </c>
       <c r="K145">
-        <v>9039</v>
+        <v>8946</v>
       </c>
       <c r="M145" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N145" t="s">
-        <v>129</v>
+      <c r="N145" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
@@ -5111,13 +5114,13 @@
         <v>202</v>
       </c>
       <c r="K146">
-        <v>9060</v>
+        <v>9039</v>
       </c>
       <c r="M146" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N146" t="s">
-        <v>130</v>
+      <c r="N146" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -5143,13 +5146,13 @@
         <v>202</v>
       </c>
       <c r="K147">
-        <v>9087</v>
+        <v>9060</v>
       </c>
       <c r="M147" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N147" t="s">
-        <v>131</v>
+      <c r="N147" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -5175,13 +5178,13 @@
         <v>202</v>
       </c>
       <c r="K148">
-        <v>9089</v>
+        <v>9087</v>
       </c>
       <c r="M148" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N148" t="s">
-        <v>132</v>
+      <c r="N148" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
@@ -5207,13 +5210,13 @@
         <v>202</v>
       </c>
       <c r="K149">
-        <v>9281</v>
+        <v>9089</v>
       </c>
       <c r="M149" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N149" t="s">
-        <v>133</v>
+      <c r="N149" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -5239,13 +5242,13 @@
         <v>202</v>
       </c>
       <c r="K150">
-        <v>9401</v>
+        <v>9281</v>
       </c>
       <c r="M150" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N150" t="s">
-        <v>134</v>
+      <c r="N150" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -5271,13 +5274,13 @@
         <v>202</v>
       </c>
       <c r="K151">
-        <v>9538</v>
+        <v>9401</v>
       </c>
       <c r="M151" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N151" t="s">
-        <v>135</v>
+      <c r="N151" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
@@ -5303,13 +5306,13 @@
         <v>202</v>
       </c>
       <c r="K152">
-        <v>9623</v>
+        <v>9538</v>
       </c>
       <c r="M152" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N152" t="s">
-        <v>136</v>
+      <c r="N152" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
@@ -5335,13 +5338,13 @@
         <v>202</v>
       </c>
       <c r="K153">
-        <v>9728</v>
+        <v>9623</v>
       </c>
       <c r="M153" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N153" t="s">
-        <v>137</v>
+      <c r="N153" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
@@ -5367,13 +5370,13 @@
         <v>202</v>
       </c>
       <c r="K154">
-        <v>10027</v>
+        <v>9728</v>
       </c>
       <c r="M154" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N154" t="s">
-        <v>138</v>
+      <c r="N154" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.25">
@@ -5399,13 +5402,13 @@
         <v>202</v>
       </c>
       <c r="K155">
-        <v>10030</v>
+        <v>10027</v>
       </c>
       <c r="M155" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N155" t="s">
-        <v>139</v>
+      <c r="N155" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
@@ -5431,13 +5434,13 @@
         <v>202</v>
       </c>
       <c r="K156">
-        <v>10067</v>
+        <v>10030</v>
       </c>
       <c r="M156" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N156" t="s">
-        <v>140</v>
+      <c r="N156" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
@@ -5463,13 +5466,13 @@
         <v>202</v>
       </c>
       <c r="K157">
-        <v>12337</v>
+        <v>10067</v>
       </c>
       <c r="M157" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N157" t="s">
-        <v>141</v>
+      <c r="N157" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
@@ -5495,13 +5498,13 @@
         <v>202</v>
       </c>
       <c r="K158">
-        <v>12394</v>
+        <v>12337</v>
       </c>
       <c r="M158" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N158" t="s">
-        <v>142</v>
+      <c r="N158" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
@@ -5527,13 +5530,13 @@
         <v>202</v>
       </c>
       <c r="K159">
-        <v>10225</v>
+        <v>12394</v>
       </c>
       <c r="M159" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N159" t="s">
-        <v>143</v>
+      <c r="N159" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
@@ -5559,13 +5562,13 @@
         <v>202</v>
       </c>
       <c r="K160">
-        <v>10385</v>
+        <v>10225</v>
       </c>
       <c r="M160" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N160" t="s">
-        <v>144</v>
+      <c r="N160" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
@@ -5591,13 +5594,13 @@
         <v>202</v>
       </c>
       <c r="K161">
-        <v>10463</v>
+        <v>10385</v>
       </c>
       <c r="M161" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N161" t="s">
-        <v>145</v>
+      <c r="N161" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
@@ -5623,13 +5626,13 @@
         <v>202</v>
       </c>
       <c r="K162">
-        <v>10500</v>
+        <v>10463</v>
       </c>
       <c r="M162" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N162" t="s">
-        <v>146</v>
+      <c r="N162" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
@@ -5655,13 +5658,13 @@
         <v>202</v>
       </c>
       <c r="K163">
-        <v>10857</v>
+        <v>10500</v>
       </c>
       <c r="M163" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N163" t="s">
-        <v>147</v>
+      <c r="N163" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
@@ -5687,13 +5690,13 @@
         <v>202</v>
       </c>
       <c r="K164">
-        <v>10877</v>
+        <v>10857</v>
       </c>
       <c r="M164" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N164" t="s">
-        <v>148</v>
+      <c r="N164" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
@@ -5719,13 +5722,13 @@
         <v>202</v>
       </c>
       <c r="K165">
-        <v>11228</v>
+        <v>10877</v>
       </c>
       <c r="M165" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N165" t="s">
-        <v>149</v>
+      <c r="N165" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
@@ -5751,13 +5754,13 @@
         <v>202</v>
       </c>
       <c r="K166">
-        <v>11632</v>
+        <v>11228</v>
       </c>
       <c r="M166" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N166" t="s">
-        <v>150</v>
+      <c r="N166" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
@@ -5783,13 +5786,13 @@
         <v>202</v>
       </c>
       <c r="K167">
-        <v>11699</v>
+        <v>11632</v>
       </c>
       <c r="M167" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N167" t="s">
-        <v>151</v>
+      <c r="N167" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
@@ -5815,13 +5818,13 @@
         <v>202</v>
       </c>
       <c r="K168">
-        <v>12458</v>
+        <v>11699</v>
       </c>
       <c r="M168" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N168" t="s">
-        <v>152</v>
+      <c r="N168" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.25">
@@ -5847,13 +5850,13 @@
         <v>202</v>
       </c>
       <c r="K169">
-        <v>12482</v>
+        <v>12458</v>
       </c>
       <c r="M169" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N169" t="s">
-        <v>153</v>
+      <c r="N169" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.25">
@@ -5879,13 +5882,13 @@
         <v>202</v>
       </c>
       <c r="K170">
-        <v>12614</v>
+        <v>12482</v>
       </c>
       <c r="M170" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N170" t="s">
-        <v>154</v>
+      <c r="N170" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
@@ -5910,14 +5913,14 @@
       <c r="J171" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K171" s="2">
-        <v>12701</v>
+      <c r="K171">
+        <v>12614</v>
       </c>
       <c r="M171" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N171" t="s">
-        <v>155</v>
+      <c r="N171" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
@@ -5943,13 +5946,13 @@
         <v>202</v>
       </c>
       <c r="K172" s="2">
-        <v>12702</v>
+        <v>12701</v>
       </c>
       <c r="M172" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N172" t="s">
-        <v>156</v>
+      <c r="N172" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
@@ -5975,13 +5978,13 @@
         <v>202</v>
       </c>
       <c r="K173" s="2">
-        <v>12703</v>
+        <v>12702</v>
       </c>
       <c r="M173" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N173" t="s">
-        <v>157</v>
+      <c r="N173" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
@@ -6007,13 +6010,13 @@
         <v>202</v>
       </c>
       <c r="K174" s="2">
-        <v>12704</v>
+        <v>12703</v>
       </c>
       <c r="M174" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N174" t="s">
-        <v>158</v>
+      <c r="N174" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
@@ -6039,13 +6042,13 @@
         <v>202</v>
       </c>
       <c r="K175" s="2">
-        <v>12705</v>
+        <v>12704</v>
       </c>
       <c r="M175" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N175" t="s">
-        <v>159</v>
+      <c r="N175" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
@@ -6071,13 +6074,13 @@
         <v>202</v>
       </c>
       <c r="K176" s="2">
-        <v>13071</v>
+        <v>12705</v>
       </c>
       <c r="M176" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N176" t="s">
-        <v>160</v>
+      <c r="N176" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.25">
@@ -6103,13 +6106,13 @@
         <v>202</v>
       </c>
       <c r="K177" s="2">
-        <v>13077</v>
+        <v>13071</v>
       </c>
       <c r="M177" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N177" t="s">
-        <v>161</v>
+      <c r="N177" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.25">
@@ -6135,13 +6138,13 @@
         <v>202</v>
       </c>
       <c r="K178" s="2">
-        <v>13082</v>
+        <v>13077</v>
       </c>
       <c r="M178" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N178" t="s">
-        <v>162</v>
+      <c r="N178" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
@@ -6167,13 +6170,13 @@
         <v>202</v>
       </c>
       <c r="K179" s="2">
-        <v>13083</v>
+        <v>13082</v>
       </c>
       <c r="M179" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N179" t="s">
-        <v>163</v>
+      <c r="N179" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.25">
@@ -6199,13 +6202,13 @@
         <v>202</v>
       </c>
       <c r="K180" s="2">
-        <v>13344</v>
+        <v>13083</v>
       </c>
       <c r="M180" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N180" t="s">
-        <v>164</v>
+      <c r="N180" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.25">
@@ -6231,13 +6234,13 @@
         <v>202</v>
       </c>
       <c r="K181" s="2">
-        <v>13342</v>
+        <v>13344</v>
       </c>
       <c r="M181" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N181" t="s">
-        <v>165</v>
+      <c r="N181" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.25">
@@ -6263,13 +6266,13 @@
         <v>202</v>
       </c>
       <c r="K182" s="2">
-        <v>13529</v>
+        <v>13342</v>
       </c>
       <c r="M182" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N182" t="s">
-        <v>166</v>
+      <c r="N182" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.25">
@@ -6295,13 +6298,13 @@
         <v>202</v>
       </c>
       <c r="K183" s="2">
-        <v>13537</v>
+        <v>13529</v>
       </c>
       <c r="M183" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N183" t="s">
-        <v>167</v>
+      <c r="N183" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.25">
@@ -6327,13 +6330,13 @@
         <v>202</v>
       </c>
       <c r="K184" s="2">
-        <v>13550</v>
+        <v>13537</v>
       </c>
       <c r="M184" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N184" t="s">
-        <v>168</v>
+      <c r="N184" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.25">
@@ -6359,13 +6362,13 @@
         <v>202</v>
       </c>
       <c r="K185" s="2">
-        <v>13572</v>
+        <v>13550</v>
       </c>
       <c r="M185" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N185" t="s">
-        <v>169</v>
+      <c r="N185" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.25">
@@ -6391,13 +6394,13 @@
         <v>202</v>
       </c>
       <c r="K186" s="2">
-        <v>13798</v>
+        <v>13572</v>
       </c>
       <c r="M186" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N186" t="s">
-        <v>170</v>
+      <c r="N186" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.25">
@@ -6423,51 +6426,45 @@
         <v>202</v>
       </c>
       <c r="K187" s="2">
-        <v>13810</v>
+        <v>13798</v>
       </c>
       <c r="M187" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N187" t="s">
-        <v>171</v>
+      <c r="N187" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B188" t="s">
         <v>21</v>
       </c>
       <c r="C188" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D188" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E188" t="s">
-        <v>23</v>
-      </c>
-      <c r="F188" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I188" t="s">
-        <v>24</v>
-      </c>
-      <c r="J188">
-        <v>25</v>
-      </c>
-      <c r="K188" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L188" t="s">
-        <v>173</v>
+        <v>18</v>
+      </c>
+      <c r="J188" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K188" s="2">
+        <v>13810</v>
       </c>
       <c r="M188" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N188" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.25">
@@ -6493,13 +6490,13 @@
         <v>24</v>
       </c>
       <c r="J189">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="K189" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L189" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M189" s="1" t="s">
         <v>22</v>
@@ -6531,13 +6528,13 @@
         <v>24</v>
       </c>
       <c r="J190">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="K190" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L190" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M190" s="1" t="s">
         <v>22</v>
@@ -6569,13 +6566,13 @@
         <v>24</v>
       </c>
       <c r="J191">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="K191" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L191" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M191" s="1" t="s">
         <v>22</v>
@@ -6607,13 +6604,13 @@
         <v>24</v>
       </c>
       <c r="J192">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="K192" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L192" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="M192" s="1" t="s">
         <v>22</v>
@@ -6683,13 +6680,13 @@
         <v>24</v>
       </c>
       <c r="J194">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="K194" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L194" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="M194" s="1" t="s">
         <v>22</v>
@@ -6759,13 +6756,13 @@
         <v>24</v>
       </c>
       <c r="J196">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="K196" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L196" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M196" s="1" t="s">
         <v>22</v>
@@ -6835,13 +6832,13 @@
         <v>24</v>
       </c>
       <c r="J198">
-        <v>333</v>
+        <v>144</v>
       </c>
       <c r="K198" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L198" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M198" s="1" t="s">
         <v>22</v>
@@ -6873,13 +6870,13 @@
         <v>24</v>
       </c>
       <c r="J199">
-        <v>623</v>
+        <v>333</v>
       </c>
       <c r="K199" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L199" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M199" s="1" t="s">
         <v>22</v>
@@ -6911,13 +6908,13 @@
         <v>24</v>
       </c>
       <c r="J200">
-        <v>987</v>
+        <v>623</v>
       </c>
       <c r="K200" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L200" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M200" s="1" t="s">
         <v>22</v>
@@ -6987,13 +6984,13 @@
         <v>24</v>
       </c>
       <c r="J202">
-        <v>1748</v>
+        <v>987</v>
       </c>
       <c r="K202" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L202" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M202" s="1" t="s">
         <v>22</v>
@@ -7101,13 +7098,13 @@
         <v>24</v>
       </c>
       <c r="J205">
-        <v>2187</v>
+        <v>1748</v>
       </c>
       <c r="K205" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L205" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M205" s="1" t="s">
         <v>22</v>
@@ -7177,13 +7174,13 @@
         <v>24</v>
       </c>
       <c r="J207">
-        <v>2824</v>
+        <v>2187</v>
       </c>
       <c r="K207" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L207" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="M207" s="1" t="s">
         <v>22</v>
@@ -7291,13 +7288,13 @@
         <v>24</v>
       </c>
       <c r="J210">
-        <v>2886</v>
+        <v>2824</v>
       </c>
       <c r="K210" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L210" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M210" s="1" t="s">
         <v>22</v>
@@ -7329,7 +7326,7 @@
         <v>24</v>
       </c>
       <c r="J211">
-        <v>2887</v>
+        <v>2886</v>
       </c>
       <c r="K211" s="1" t="s">
         <v>203</v>
@@ -7367,7 +7364,7 @@
         <v>24</v>
       </c>
       <c r="J212">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="K212" s="1" t="s">
         <v>203</v>
@@ -7405,7 +7402,7 @@
         <v>24</v>
       </c>
       <c r="J213">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="K213" s="1" t="s">
         <v>203</v>
@@ -7443,13 +7440,13 @@
         <v>24</v>
       </c>
       <c r="J214">
-        <v>3338</v>
+        <v>2889</v>
       </c>
       <c r="K214" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L214" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="M214" s="1" t="s">
         <v>22</v>
@@ -7519,13 +7516,13 @@
         <v>24</v>
       </c>
       <c r="J216">
-        <v>3462</v>
+        <v>3338</v>
       </c>
       <c r="K216" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L216" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M216" s="1" t="s">
         <v>22</v>
@@ -7671,13 +7668,13 @@
         <v>24</v>
       </c>
       <c r="J220">
-        <v>4069</v>
+        <v>3462</v>
       </c>
       <c r="K220" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L220" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M220" s="1" t="s">
         <v>22</v>
@@ -7709,13 +7706,13 @@
         <v>24</v>
       </c>
       <c r="J221">
-        <v>4404</v>
+        <v>4069</v>
       </c>
       <c r="K221" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L221" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M221" s="1" t="s">
         <v>22</v>
@@ -8089,13 +8086,13 @@
         <v>24</v>
       </c>
       <c r="J231">
-        <v>4817</v>
+        <v>4404</v>
       </c>
       <c r="K231" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L231" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M231" s="1" t="s">
         <v>22</v>
@@ -8127,13 +8124,13 @@
         <v>24</v>
       </c>
       <c r="J232">
-        <v>5194</v>
+        <v>4817</v>
       </c>
       <c r="K232" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L232" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M232" s="1" t="s">
         <v>22</v>
@@ -8165,13 +8162,13 @@
         <v>24</v>
       </c>
       <c r="J233">
-        <v>5198</v>
+        <v>5194</v>
       </c>
       <c r="K233" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L233" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M233" s="1" t="s">
         <v>22</v>
@@ -8203,13 +8200,13 @@
         <v>24</v>
       </c>
       <c r="J234">
-        <v>5466</v>
+        <v>5198</v>
       </c>
       <c r="K234" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L234" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M234" s="1" t="s">
         <v>22</v>
@@ -8279,13 +8276,13 @@
         <v>24</v>
       </c>
       <c r="J236">
-        <v>5482</v>
+        <v>5466</v>
       </c>
       <c r="K236" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L236" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="M236" s="1" t="s">
         <v>22</v>
@@ -8393,7 +8390,7 @@
         <v>24</v>
       </c>
       <c r="J239">
-        <v>5483</v>
+        <v>5482</v>
       </c>
       <c r="K239" s="1" t="s">
         <v>203</v>
@@ -8507,7 +8504,7 @@
         <v>24</v>
       </c>
       <c r="J242">
-        <v>5484</v>
+        <v>5483</v>
       </c>
       <c r="K242" s="1" t="s">
         <v>203</v>
@@ -8621,7 +8618,7 @@
         <v>24</v>
       </c>
       <c r="J245">
-        <v>5485</v>
+        <v>5484</v>
       </c>
       <c r="K245" s="1" t="s">
         <v>203</v>
@@ -8735,13 +8732,13 @@
         <v>24</v>
       </c>
       <c r="J248">
-        <v>5534</v>
+        <v>5485</v>
       </c>
       <c r="K248" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L248" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M248" s="1" t="s">
         <v>22</v>
@@ -8811,7 +8808,7 @@
         <v>24</v>
       </c>
       <c r="J250">
-        <v>5535</v>
+        <v>5534</v>
       </c>
       <c r="K250" s="1" t="s">
         <v>203</v>
@@ -8887,13 +8884,13 @@
         <v>24</v>
       </c>
       <c r="J252">
-        <v>5790</v>
+        <v>5535</v>
       </c>
       <c r="K252" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L252" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M252" s="1" t="s">
         <v>22</v>
@@ -8925,13 +8922,13 @@
         <v>24</v>
       </c>
       <c r="J253">
-        <v>5835</v>
+        <v>5790</v>
       </c>
       <c r="K253" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L253" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="M253" s="1" t="s">
         <v>22</v>
@@ -9001,13 +8998,13 @@
         <v>24</v>
       </c>
       <c r="J255">
-        <v>5838</v>
+        <v>5835</v>
       </c>
       <c r="K255" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L255" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="M255" s="1" t="s">
         <v>22</v>
@@ -9115,13 +9112,13 @@
         <v>24</v>
       </c>
       <c r="J258">
-        <v>5855</v>
+        <v>5838</v>
       </c>
       <c r="K258" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L258" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="M258" s="1" t="s">
         <v>22</v>
@@ -9191,7 +9188,7 @@
         <v>24</v>
       </c>
       <c r="J260">
-        <v>5856</v>
+        <v>5855</v>
       </c>
       <c r="K260" s="1" t="s">
         <v>203</v>
@@ -9419,13 +9416,13 @@
         <v>24</v>
       </c>
       <c r="J266">
-        <v>5959</v>
+        <v>5856</v>
       </c>
       <c r="K266" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L266" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="M266" s="1" t="s">
         <v>22</v>
@@ -9457,13 +9454,13 @@
         <v>24</v>
       </c>
       <c r="J267">
-        <v>6009</v>
+        <v>5959</v>
       </c>
       <c r="K267" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L267" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="M267" s="1" t="s">
         <v>22</v>
@@ -9571,13 +9568,13 @@
         <v>24</v>
       </c>
       <c r="J270">
-        <v>6202</v>
+        <v>6009</v>
       </c>
       <c r="K270" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L270" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M270" s="1" t="s">
         <v>22</v>
@@ -9609,13 +9606,13 @@
         <v>24</v>
       </c>
       <c r="J271">
-        <v>6334</v>
+        <v>6202</v>
       </c>
       <c r="K271" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L271" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M271" s="1" t="s">
         <v>22</v>
@@ -9685,13 +9682,13 @@
         <v>24</v>
       </c>
       <c r="J273">
-        <v>6724</v>
+        <v>6334</v>
       </c>
       <c r="K273" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L273" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="M273" s="1" t="s">
         <v>22</v>
@@ -9723,13 +9720,13 @@
         <v>24</v>
       </c>
       <c r="J274">
-        <v>6726</v>
+        <v>6724</v>
       </c>
       <c r="K274" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L274" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M274" s="1" t="s">
         <v>22</v>
@@ -9761,13 +9758,13 @@
         <v>24</v>
       </c>
       <c r="J275">
-        <v>6893</v>
+        <v>6726</v>
       </c>
       <c r="K275" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L275" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="M275" s="1" t="s">
         <v>22</v>
@@ -9837,13 +9834,13 @@
         <v>24</v>
       </c>
       <c r="J277">
-        <v>7299</v>
+        <v>6893</v>
       </c>
       <c r="K277" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L277" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M277" s="1" t="s">
         <v>22</v>
@@ -9875,13 +9872,13 @@
         <v>24</v>
       </c>
       <c r="J278">
-        <v>7702</v>
+        <v>7299</v>
       </c>
       <c r="K278" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L278" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="M278" s="1" t="s">
         <v>22</v>
@@ -9989,13 +9986,13 @@
         <v>24</v>
       </c>
       <c r="J281">
-        <v>7756</v>
+        <v>7702</v>
       </c>
       <c r="K281" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L281" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="M281" s="1" t="s">
         <v>22</v>
@@ -10141,13 +10138,13 @@
         <v>24</v>
       </c>
       <c r="J285">
-        <v>7793</v>
+        <v>7756</v>
       </c>
       <c r="K285" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L285" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M285" s="1" t="s">
         <v>22</v>
@@ -10217,7 +10214,7 @@
         <v>24</v>
       </c>
       <c r="J287">
-        <v>7794</v>
+        <v>7793</v>
       </c>
       <c r="K287" s="1" t="s">
         <v>203</v>
@@ -10293,7 +10290,7 @@
         <v>24</v>
       </c>
       <c r="J289">
-        <v>7795</v>
+        <v>7794</v>
       </c>
       <c r="K289" s="1" t="s">
         <v>203</v>
@@ -10369,7 +10366,7 @@
         <v>24</v>
       </c>
       <c r="J291">
-        <v>7796</v>
+        <v>7795</v>
       </c>
       <c r="K291" s="1" t="s">
         <v>203</v>
@@ -10445,7 +10442,7 @@
         <v>24</v>
       </c>
       <c r="J293">
-        <v>7798</v>
+        <v>7796</v>
       </c>
       <c r="K293" s="1" t="s">
         <v>203</v>
@@ -10673,13 +10670,13 @@
         <v>24</v>
       </c>
       <c r="J299">
-        <v>7888</v>
+        <v>7798</v>
       </c>
       <c r="K299" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L299" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="M299" s="1" t="s">
         <v>22</v>
@@ -10787,7 +10784,7 @@
         <v>24</v>
       </c>
       <c r="J302">
-        <v>7889</v>
+        <v>7888</v>
       </c>
       <c r="K302" s="1" t="s">
         <v>203</v>
@@ -10863,13 +10860,13 @@
         <v>24</v>
       </c>
       <c r="J304">
-        <v>7977</v>
+        <v>7889</v>
       </c>
       <c r="K304" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L304" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M304" s="1" t="s">
         <v>22</v>
@@ -10977,13 +10974,13 @@
         <v>24</v>
       </c>
       <c r="J307">
-        <v>8049</v>
+        <v>7977</v>
       </c>
       <c r="K307" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L307" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="M307" s="1" t="s">
         <v>22</v>
@@ -11015,7 +11012,7 @@
         <v>24</v>
       </c>
       <c r="J308">
-        <v>8054</v>
+        <v>8049</v>
       </c>
       <c r="K308" s="1" t="s">
         <v>203</v>
@@ -11129,7 +11126,7 @@
         <v>24</v>
       </c>
       <c r="J311">
-        <v>8055</v>
+        <v>8054</v>
       </c>
       <c r="K311" s="1" t="s">
         <v>203</v>
@@ -11243,7 +11240,7 @@
         <v>24</v>
       </c>
       <c r="J314">
-        <v>8056</v>
+        <v>8055</v>
       </c>
       <c r="K314" s="1" t="s">
         <v>203</v>
@@ -11281,7 +11278,7 @@
         <v>24</v>
       </c>
       <c r="J315">
-        <v>8057</v>
+        <v>8056</v>
       </c>
       <c r="K315" s="1" t="s">
         <v>203</v>
@@ -11357,7 +11354,7 @@
         <v>24</v>
       </c>
       <c r="J317">
-        <v>8058</v>
+        <v>8057</v>
       </c>
       <c r="K317" s="1" t="s">
         <v>203</v>
@@ -11433,7 +11430,7 @@
         <v>24</v>
       </c>
       <c r="J319">
-        <v>8059</v>
+        <v>8058</v>
       </c>
       <c r="K319" s="1" t="s">
         <v>203</v>
@@ -11471,7 +11468,7 @@
         <v>24</v>
       </c>
       <c r="J320">
-        <v>8060</v>
+        <v>8059</v>
       </c>
       <c r="K320" s="1" t="s">
         <v>203</v>
@@ -11623,7 +11620,7 @@
         <v>24</v>
       </c>
       <c r="J324">
-        <v>8061</v>
+        <v>8060</v>
       </c>
       <c r="K324" s="1" t="s">
         <v>203</v>
@@ -11927,7 +11924,7 @@
         <v>24</v>
       </c>
       <c r="J332">
-        <v>8062</v>
+        <v>8061</v>
       </c>
       <c r="K332" s="1" t="s">
         <v>203</v>
@@ -11965,7 +11962,7 @@
         <v>24</v>
       </c>
       <c r="J333">
-        <v>8063</v>
+        <v>8062</v>
       </c>
       <c r="K333" s="1" t="s">
         <v>203</v>
@@ -12041,7 +12038,7 @@
         <v>24</v>
       </c>
       <c r="J335">
-        <v>8064</v>
+        <v>8063</v>
       </c>
       <c r="K335" s="1" t="s">
         <v>203</v>
@@ -12079,7 +12076,7 @@
         <v>24</v>
       </c>
       <c r="J336">
-        <v>8065</v>
+        <v>8064</v>
       </c>
       <c r="K336" s="1" t="s">
         <v>203</v>
@@ -12155,7 +12152,7 @@
         <v>24</v>
       </c>
       <c r="J338">
-        <v>8066</v>
+        <v>8065</v>
       </c>
       <c r="K338" s="1" t="s">
         <v>203</v>
@@ -12307,13 +12304,13 @@
         <v>24</v>
       </c>
       <c r="J342">
-        <v>8112</v>
+        <v>8066</v>
       </c>
       <c r="K342" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L342" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="M342" s="1" t="s">
         <v>22</v>
@@ -12345,7 +12342,7 @@
         <v>24</v>
       </c>
       <c r="J343">
-        <v>8113</v>
+        <v>8112</v>
       </c>
       <c r="K343" s="1" t="s">
         <v>203</v>
@@ -12383,7 +12380,7 @@
         <v>24</v>
       </c>
       <c r="J344">
-        <v>8114</v>
+        <v>8113</v>
       </c>
       <c r="K344" s="1" t="s">
         <v>203</v>
@@ -12421,7 +12418,7 @@
         <v>24</v>
       </c>
       <c r="J345">
-        <v>8115</v>
+        <v>8114</v>
       </c>
       <c r="K345" s="1" t="s">
         <v>203</v>
@@ -12459,7 +12456,7 @@
         <v>24</v>
       </c>
       <c r="J346">
-        <v>8116</v>
+        <v>8115</v>
       </c>
       <c r="K346" s="1" t="s">
         <v>203</v>
@@ -12497,13 +12494,13 @@
         <v>24</v>
       </c>
       <c r="J347">
-        <v>8255</v>
+        <v>8116</v>
       </c>
       <c r="K347" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L347" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="M347" s="1" t="s">
         <v>22</v>
@@ -12535,13 +12532,13 @@
         <v>24</v>
       </c>
       <c r="J348">
-        <v>8481</v>
+        <v>8255</v>
       </c>
       <c r="K348" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L348" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M348" s="1" t="s">
         <v>22</v>
@@ -12649,13 +12646,13 @@
         <v>24</v>
       </c>
       <c r="J351">
-        <v>8678</v>
+        <v>8481</v>
       </c>
       <c r="K351" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L351" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M351" s="1" t="s">
         <v>22</v>
@@ -12801,7 +12798,7 @@
         <v>24</v>
       </c>
       <c r="J355">
-        <v>8679</v>
+        <v>8678</v>
       </c>
       <c r="K355" s="1" t="s">
         <v>203</v>
@@ -12953,13 +12950,13 @@
         <v>24</v>
       </c>
       <c r="J359">
-        <v>8684</v>
+        <v>8679</v>
       </c>
       <c r="K359" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L359" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="M359" s="1" t="s">
         <v>22</v>
@@ -13029,13 +13026,13 @@
         <v>24</v>
       </c>
       <c r="J361">
-        <v>8691</v>
+        <v>8684</v>
       </c>
       <c r="K361" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L361" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M361" s="1" t="s">
         <v>22</v>
@@ -13067,13 +13064,13 @@
         <v>24</v>
       </c>
       <c r="J362">
-        <v>9114</v>
+        <v>8691</v>
       </c>
       <c r="K362" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L362" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M362" s="1" t="s">
         <v>22</v>
@@ -13219,7 +13216,7 @@
         <v>24</v>
       </c>
       <c r="J366">
-        <v>9121</v>
+        <v>9114</v>
       </c>
       <c r="K366" s="1" t="s">
         <v>203</v>
@@ -13333,13 +13330,13 @@
         <v>24</v>
       </c>
       <c r="J369">
-        <v>9139</v>
+        <v>9121</v>
       </c>
       <c r="K369" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L369" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="M369" s="1" t="s">
         <v>22</v>
@@ -13485,7 +13482,7 @@
         <v>24</v>
       </c>
       <c r="J373">
-        <v>9140</v>
+        <v>9139</v>
       </c>
       <c r="K373" s="1" t="s">
         <v>203</v>
@@ -13561,7 +13558,7 @@
         <v>24</v>
       </c>
       <c r="J375">
-        <v>9141</v>
+        <v>9140</v>
       </c>
       <c r="K375" s="1" t="s">
         <v>203</v>
@@ -13605,7 +13602,7 @@
         <v>203</v>
       </c>
       <c r="L376" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="M376" s="1" t="s">
         <v>22</v>
@@ -13751,7 +13748,7 @@
         <v>24</v>
       </c>
       <c r="J380">
-        <v>9142</v>
+        <v>9141</v>
       </c>
       <c r="K380" s="1" t="s">
         <v>203</v>
@@ -13865,7 +13862,7 @@
         <v>24</v>
       </c>
       <c r="J383">
-        <v>9143</v>
+        <v>9142</v>
       </c>
       <c r="K383" s="1" t="s">
         <v>203</v>
@@ -13979,13 +13976,13 @@
         <v>24</v>
       </c>
       <c r="J386">
-        <v>9298</v>
+        <v>9143</v>
       </c>
       <c r="K386" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L386" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="M386" s="1" t="s">
         <v>22</v>
@@ -14169,13 +14166,13 @@
         <v>24</v>
       </c>
       <c r="J391">
-        <v>9373</v>
+        <v>9298</v>
       </c>
       <c r="K391" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L391" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M391" s="1" t="s">
         <v>22</v>
@@ -14207,13 +14204,13 @@
         <v>24</v>
       </c>
       <c r="J392">
-        <v>9394</v>
+        <v>9373</v>
       </c>
       <c r="K392" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L392" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="M392" s="1" t="s">
         <v>22</v>
@@ -14245,7 +14242,7 @@
         <v>24</v>
       </c>
       <c r="J393">
-        <v>9395</v>
+        <v>9394</v>
       </c>
       <c r="K393" s="1" t="s">
         <v>203</v>
@@ -14283,13 +14280,13 @@
         <v>24</v>
       </c>
       <c r="J394">
-        <v>9639</v>
+        <v>9395</v>
       </c>
       <c r="K394" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L394" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M394" s="1" t="s">
         <v>22</v>
@@ -14321,7 +14318,7 @@
         <v>24</v>
       </c>
       <c r="J395">
-        <v>9640</v>
+        <v>9639</v>
       </c>
       <c r="K395" s="1" t="s">
         <v>203</v>
@@ -14435,13 +14432,13 @@
         <v>24</v>
       </c>
       <c r="J398">
-        <v>9687</v>
+        <v>9640</v>
       </c>
       <c r="K398" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L398" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="M398" s="1" t="s">
         <v>22</v>
@@ -14549,13 +14546,13 @@
         <v>24</v>
       </c>
       <c r="J401">
-        <v>9766</v>
+        <v>9687</v>
       </c>
       <c r="K401" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L401" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="M401" s="1" t="s">
         <v>22</v>
@@ -14701,7 +14698,7 @@
         <v>24</v>
       </c>
       <c r="J405">
-        <v>9767</v>
+        <v>9766</v>
       </c>
       <c r="K405" s="1" t="s">
         <v>203</v>
@@ -14777,7 +14774,7 @@
         <v>24</v>
       </c>
       <c r="J407">
-        <v>9771</v>
+        <v>9767</v>
       </c>
       <c r="K407" s="1" t="s">
         <v>203</v>
@@ -15043,13 +15040,13 @@
         <v>24</v>
       </c>
       <c r="J414">
-        <v>9827</v>
+        <v>9771</v>
       </c>
       <c r="K414" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L414" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M414" s="1" t="s">
         <v>22</v>
@@ -15157,13 +15154,13 @@
         <v>24</v>
       </c>
       <c r="J417">
-        <v>9917</v>
+        <v>9827</v>
       </c>
       <c r="K417" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L417" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M417" s="1" t="s">
         <v>22</v>
@@ -15385,13 +15382,13 @@
         <v>24</v>
       </c>
       <c r="J423">
-        <v>9965</v>
+        <v>9917</v>
       </c>
       <c r="K423" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L423" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="M423" s="1" t="s">
         <v>22</v>
@@ -15461,13 +15458,13 @@
         <v>24</v>
       </c>
       <c r="J425">
-        <v>9999</v>
+        <v>9965</v>
       </c>
       <c r="K425" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L425" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="M425" s="1" t="s">
         <v>22</v>
@@ -15537,13 +15534,13 @@
         <v>24</v>
       </c>
       <c r="J427">
-        <v>12337</v>
+        <v>9999</v>
       </c>
       <c r="K427" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L427" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M427" s="1" t="s">
         <v>22</v>
@@ -15613,13 +15610,13 @@
         <v>24</v>
       </c>
       <c r="J429">
-        <v>12382</v>
+        <v>12337</v>
       </c>
       <c r="K429" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L429" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M429" s="1" t="s">
         <v>22</v>
@@ -15651,7 +15648,7 @@
         <v>24</v>
       </c>
       <c r="J430">
-        <v>12404</v>
+        <v>12382</v>
       </c>
       <c r="K430" s="1" t="s">
         <v>203</v>
@@ -15689,13 +15686,13 @@
         <v>24</v>
       </c>
       <c r="J431">
-        <v>10394</v>
+        <v>12404</v>
       </c>
       <c r="K431" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L431" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="M431" s="1" t="s">
         <v>22</v>
@@ -15727,13 +15724,13 @@
         <v>24</v>
       </c>
       <c r="J432">
-        <v>10500</v>
+        <v>10394</v>
       </c>
       <c r="K432" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L432" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="M432" s="1" t="s">
         <v>22</v>
@@ -15841,7 +15838,7 @@
         <v>24</v>
       </c>
       <c r="J435">
-        <v>10877</v>
+        <v>10500</v>
       </c>
       <c r="K435" s="1" t="s">
         <v>203</v>
@@ -15879,13 +15876,13 @@
         <v>24</v>
       </c>
       <c r="J436">
-        <v>10894</v>
+        <v>10877</v>
       </c>
       <c r="K436" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L436" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="M436" s="1" t="s">
         <v>22</v>
@@ -15917,13 +15914,13 @@
         <v>24</v>
       </c>
       <c r="J437">
-        <v>10914</v>
+        <v>10894</v>
       </c>
       <c r="K437" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L437" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="M437" s="1" t="s">
         <v>22</v>
@@ -15955,13 +15952,13 @@
         <v>24</v>
       </c>
       <c r="J438">
-        <v>11258</v>
+        <v>10914</v>
       </c>
       <c r="K438" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L438" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M438" s="1" t="s">
         <v>22</v>
@@ -15993,13 +15990,13 @@
         <v>24</v>
       </c>
       <c r="J439">
-        <v>11744</v>
+        <v>11258</v>
       </c>
       <c r="K439" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L439" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="M439" s="1" t="s">
         <v>22</v>
@@ -16069,13 +16066,13 @@
         <v>24</v>
       </c>
       <c r="J441">
-        <v>12095</v>
+        <v>11744</v>
       </c>
       <c r="K441" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L441" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M441" s="1" t="s">
         <v>22</v>
@@ -16107,13 +16104,13 @@
         <v>24</v>
       </c>
       <c r="J442">
-        <v>12151</v>
+        <v>12095</v>
       </c>
       <c r="K442" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L442" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="M442" s="1" t="s">
         <v>22</v>
@@ -16145,13 +16142,13 @@
         <v>24</v>
       </c>
       <c r="J443">
-        <v>12182</v>
+        <v>12151</v>
       </c>
       <c r="K443" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L443" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="M443" s="1" t="s">
         <v>22</v>
@@ -16259,13 +16256,13 @@
         <v>24</v>
       </c>
       <c r="J446">
-        <v>13083</v>
+        <v>12182</v>
       </c>
       <c r="K446" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L446" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="M446" s="1" t="s">
         <v>22</v>
@@ -16373,13 +16370,13 @@
         <v>24</v>
       </c>
       <c r="J449">
-        <v>13261</v>
+        <v>13083</v>
       </c>
       <c r="K449" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L449" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="M449" s="1" t="s">
         <v>22</v>
@@ -16487,13 +16484,13 @@
         <v>24</v>
       </c>
       <c r="J452">
-        <v>13452</v>
+        <v>13261</v>
       </c>
       <c r="K452" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L452" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="M452" s="1" t="s">
         <v>22</v>
@@ -16905,13 +16902,13 @@
         <v>24</v>
       </c>
       <c r="J463">
-        <v>13846</v>
+        <v>13452</v>
       </c>
       <c r="K463" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L463" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M463" s="1" t="s">
         <v>22</v>
@@ -16981,13 +16978,13 @@
         <v>24</v>
       </c>
       <c r="J465">
-        <v>13976</v>
+        <v>13846</v>
       </c>
       <c r="K465" s="1" t="s">
         <v>203</v>
       </c>
       <c r="L465" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="M465" s="1" t="s">
         <v>22</v>
@@ -17186,8 +17183,46 @@
         <v>172</v>
       </c>
     </row>
+    <row r="471" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>206</v>
+      </c>
+      <c r="B471" t="s">
+        <v>21</v>
+      </c>
+      <c r="C471" t="s">
+        <v>25</v>
+      </c>
+      <c r="D471" t="s">
+        <v>15</v>
+      </c>
+      <c r="E471" t="s">
+        <v>23</v>
+      </c>
+      <c r="F471" t="s">
+        <v>26</v>
+      </c>
+      <c r="I471" t="s">
+        <v>24</v>
+      </c>
+      <c r="J471">
+        <v>13976</v>
+      </c>
+      <c r="K471" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L471" t="s">
+        <v>201</v>
+      </c>
+      <c r="M471" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N471" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:N470"/>
+  <autoFilter ref="B1:N471"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>